<commit_message>
Editing Ionnization of Mercury Lab
</commit_message>
<xml_diff>
--- a/Ionization of Mercury/IonizationofMercury.xlsx
+++ b/Ionization of Mercury/IonizationofMercury.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4290" windowHeight="5415" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4290" windowHeight="5415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Voltage (V)</t>
   </si>
@@ -61,19 +61,33 @@
     <t>Sub up</t>
   </si>
   <si>
-    <t>Recorded Voltage [V]</t>
-  </si>
-  <si>
-    <t>Current [mA*10^-9]</t>
-  </si>
-  <si>
-    <t>Adjusted Voltage [V]</t>
-  </si>
-  <si>
     <t>Altered Current</t>
   </si>
   <si>
     <t>Altered Voltage</t>
+  </si>
+  <si>
+    <r>
+      <t>Recorded Voltage [V] (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±0.01V)</t>
+    </r>
+  </si>
+  <si>
+    <t>Recorded Voltage [V] (±0.01V)</t>
+  </si>
+  <si>
+    <t>Adjusted Voltage [V] (±0.01V)</t>
+  </si>
+  <si>
+    <t>Current [mA*10^-9] (0.05 mA*10^-9)</t>
   </si>
 </sst>
 </file>
@@ -83,9 +97,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,13 +107,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,15 +148,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -229,7 +266,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Switch 1</c:v>
+            <c:v>Switch Position 0</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -500,7 +537,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Switch 2</c:v>
+            <c:v>Switch Position 1</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -842,6 +879,36 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Uncalibrated</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Voltage [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -934,6 +1001,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Adjusted Current [mA^(2/3)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1014,6 +1106,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21810545613519383"/>
+          <c:y val="0.34193452719152351"/>
+          <c:w val="0.15998284024031847"/>
+          <c:h val="9.224853049038749E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1783,6 +1885,44 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Calibrated Voltage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39295950055409368"/>
+              <c:y val="0.84762894005721023"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1875,6 +2015,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Adjusted Current [mA^(2/3)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2065,12 +2230,25 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-CA"/>
-              <a:t>365</a:t>
+              <a:rPr lang="en-CA" sz="1200"/>
+              <a:t>Callibrated</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" sz="1200" baseline="0"/>
+              <a:t> measrements at a wavelength of 365 nm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA" sz="1200"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10822900262467192"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2102,7 +2280,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12981714785651793"/>
+          <c:y val="0.14435185185185184"/>
+          <c:w val="0.81862729658792655"/>
+          <c:h val="0.618248031496063"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2510,6 +2698,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="900"/>
+                  <a:t>Calibrated Voltage [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2602,6 +2815,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA" sz="900"/>
+                  <a:t>Photomultiplier Current [mA*10^-9]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2682,6 +2920,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24726137357830272"/>
+          <c:y val="0.27372630504520262"/>
+          <c:w val="0.17214391951006125"/>
+          <c:h val="7.8125546806649168E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7071,15 +7319,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>50006</xdr:colOff>
+      <xdr:colOff>50005</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>164306</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>73818</xdr:colOff>
+      <xdr:colOff>280986</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>11906</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7177,6 +7425,60 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:C11" totalsRowShown="0">
+  <autoFilter ref="A3:C11">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Recorded Voltage [V] (±0.01V)"/>
+    <tableColumn id="2" name="Adjusted Voltage [V] (±0.01V)">
+      <calculatedColumnFormula>A4-2.418</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Current [mA*10^-9] (0.05 mA*10^-9)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A16:C22" totalsRowShown="0">
+  <autoFilter ref="A16:C22">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Recorded Voltage [V] (±0.01V)"/>
+    <tableColumn id="2" name="Adjusted Voltage [V] (±0.01V)">
+      <calculatedColumnFormula>A17-2.418</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Current [mA*10^-9] (0.05 mA*10^-9)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A27:C35" totalsRowShown="0">
+  <autoFilter ref="A27:C35">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Recorded Voltage [V] (±0.01V)"/>
+    <tableColumn id="2" name="Adjusted Voltage [V] (±0.01V)">
+      <calculatedColumnFormula>A28-2.418</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Current [mA*10^-9] (0.05 mA*10^-9)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7478,7 +7780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="K22" zoomScale="106" workbookViewId="0">
       <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
@@ -7518,25 +7820,25 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -7551,7 +7853,7 @@
         <v>0.83750000000000002</v>
       </c>
       <c r="D4">
-        <f>C4^(2/3)</f>
+        <f t="shared" ref="D4:D39" si="0">C4^(2/3)</f>
         <v>0.88849818260367752</v>
       </c>
       <c r="F4">
@@ -7565,7 +7867,7 @@
         <v>2.4266000000000001</v>
       </c>
       <c r="I4">
-        <f>H4^(2/3)</f>
+        <f t="shared" ref="I4:I46" si="1">H4^(2/3)</f>
         <v>1.8057825925315851</v>
       </c>
     </row>
@@ -7574,28 +7876,28 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B39" si="0">A5+2.418</f>
+        <f t="shared" ref="B5:B39" si="2">A5+2.418</f>
         <v>3.4180000000000001</v>
       </c>
       <c r="C5">
         <v>1.4303999999999999</v>
       </c>
       <c r="D5">
-        <f>C5^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>1.2695164546828319</v>
       </c>
       <c r="F5">
         <v>6.0030000000000001</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G46" si="1">F5-0.07</f>
+        <f t="shared" ref="G5:G46" si="3">F5-0.07</f>
         <v>5.9329999999999998</v>
       </c>
       <c r="H5">
         <v>3.2075</v>
       </c>
       <c r="I5">
-        <f>H5^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.1749257912761819</v>
       </c>
     </row>
@@ -7604,28 +7906,28 @@
         <v>2.0009999999999999</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.4190000000000005</v>
       </c>
       <c r="C6">
         <v>2.1160999999999999</v>
       </c>
       <c r="D6">
-        <f>C6^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>1.6482539484883461</v>
       </c>
       <c r="F6">
         <v>7.0119999999999996</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.9419999999999993</v>
       </c>
       <c r="H6">
         <v>4.0785999999999998</v>
       </c>
       <c r="I6">
-        <f>H6^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.5527448572279576</v>
       </c>
     </row>
@@ -7634,28 +7936,28 @@
         <v>3.0019999999999998</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.42</v>
       </c>
       <c r="C7">
         <v>2.8673000000000002</v>
       </c>
       <c r="D7">
-        <f>C7^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.0182831284771843</v>
       </c>
       <c r="F7">
         <v>7.1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0299999999999994</v>
       </c>
       <c r="H7">
         <v>4.1452</v>
       </c>
       <c r="I7">
-        <f>H7^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.5804591775319281</v>
       </c>
     </row>
@@ -7664,28 +7966,28 @@
         <v>4.0039999999999996</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6.4219999999999997</v>
       </c>
       <c r="C8">
         <v>3.6951999999999998</v>
       </c>
       <c r="D8">
-        <f>C8^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.3901507838320488</v>
       </c>
       <c r="F8">
         <v>7.2050000000000001</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.1349999999999998</v>
       </c>
       <c r="H8">
         <v>4.2405999999999997</v>
       </c>
       <c r="I8">
-        <f>H8^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.6199009519108367</v>
       </c>
     </row>
@@ -7694,28 +7996,28 @@
         <v>5.0019999999999998</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.42</v>
       </c>
       <c r="C9">
         <v>4.5900999999999996</v>
       </c>
       <c r="D9">
-        <f>C9^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.761943338789874</v>
       </c>
       <c r="F9">
         <v>7.3</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2299999999999995</v>
       </c>
       <c r="H9">
         <v>4.3266999999999998</v>
       </c>
       <c r="I9">
-        <f>H9^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.6552445273745451</v>
       </c>
     </row>
@@ -7724,28 +8026,28 @@
         <v>5.5</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.9180000000000001</v>
       </c>
       <c r="C10">
         <v>5.0692000000000004</v>
       </c>
       <c r="D10">
-        <f>C10^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.9509348235262696</v>
       </c>
       <c r="F10">
         <v>7.4130000000000003</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.343</v>
       </c>
       <c r="H10">
         <v>4.4333</v>
       </c>
       <c r="I10">
-        <f>H10^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.6986801454947553</v>
       </c>
     </row>
@@ -7754,28 +8056,28 @@
         <v>5.12</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5380000000000003</v>
       </c>
       <c r="C11">
         <v>4.7108999999999996</v>
       </c>
       <c r="D11">
-        <f>C11^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.810191550287843</v>
       </c>
       <c r="F11">
         <v>7.5049999999999999</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.4349999999999996</v>
       </c>
       <c r="H11">
         <v>4.5175999999999998</v>
       </c>
       <c r="I11">
-        <f>H11^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.7327832251382156</v>
       </c>
     </row>
@@ -7784,28 +8086,28 @@
         <v>5.2089999999999996</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.6269999999999998</v>
       </c>
       <c r="C12">
         <v>4.7853000000000003</v>
       </c>
       <c r="D12">
-        <f>C12^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.8397020818385852</v>
       </c>
       <c r="F12">
         <v>7.6020000000000003</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.532</v>
       </c>
       <c r="H12">
         <v>4.6079999999999997</v>
       </c>
       <c r="I12">
-        <f>H12^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.7691191749902235</v>
       </c>
     </row>
@@ -7814,28 +8116,28 @@
         <v>5.2679999999999998</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.6859999999999999</v>
       </c>
       <c r="C13">
         <v>4.8468999999999998</v>
       </c>
       <c r="D13">
-        <f>C13^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.8640199558190718</v>
       </c>
       <c r="F13">
         <v>7.7080000000000002</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.6379999999999999</v>
       </c>
       <c r="H13">
         <v>4.7054999999999998</v>
       </c>
       <c r="I13">
-        <f>H13^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.808043633048583</v>
       </c>
     </row>
@@ -7844,28 +8146,28 @@
         <v>5.4009999999999998</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.819</v>
       </c>
       <c r="C14">
         <v>4.9682000000000004</v>
       </c>
       <c r="D14">
-        <f>C14^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.9116067240118975</v>
       </c>
       <c r="F14">
         <v>7.8010000000000002</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.7309999999999999</v>
       </c>
       <c r="H14" s="2">
         <v>4.7930999999999999</v>
       </c>
       <c r="I14">
-        <f>H14^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.8427870383087122</v>
       </c>
     </row>
@@ -7874,28 +8176,28 @@
         <v>5.5910000000000002</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.0090000000000003</v>
       </c>
       <c r="C15">
         <v>5.1611000000000002</v>
       </c>
       <c r="D15">
-        <f>C15^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>2.9864931017573073</v>
       </c>
       <c r="F15">
         <v>7.9009999999999998</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.8309999999999995</v>
       </c>
       <c r="H15">
         <v>4.8912000000000004</v>
       </c>
       <c r="I15">
-        <f>H15^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.8814446455961154</v>
       </c>
       <c r="J15" s="1"/>
@@ -7905,28 +8207,28 @@
         <v>5.7039999999999997</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.1219999999999999</v>
       </c>
       <c r="C16">
         <v>5.2721</v>
       </c>
       <c r="D16">
-        <f>C16^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.0291614845071742</v>
       </c>
       <c r="F16">
         <v>8.0050000000000008</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.9350000000000005</v>
       </c>
       <c r="H16">
         <v>4.9936999999999996</v>
       </c>
       <c r="I16">
-        <f>H16^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.9215610472269788</v>
       </c>
     </row>
@@ -7935,28 +8237,28 @@
         <v>5.8049999999999997</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.222999999999999</v>
       </c>
       <c r="C17">
         <v>5.3661000000000003</v>
       </c>
       <c r="D17">
-        <f>C17^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.065061369276326</v>
       </c>
       <c r="F17">
         <v>8.1050000000000004</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.0350000000000001</v>
       </c>
       <c r="H17">
         <v>5.0883000000000003</v>
       </c>
       <c r="I17">
-        <f>H17^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.9583426353808333</v>
       </c>
     </row>
@@ -7965,28 +8267,28 @@
         <v>5.9029999999999996</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.3209999999999997</v>
       </c>
       <c r="C18">
         <v>5.4691000000000001</v>
       </c>
       <c r="D18">
-        <f>C18^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.1041586507243615</v>
       </c>
       <c r="F18">
         <v>8.1869999999999994</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.1169999999999991</v>
       </c>
       <c r="H18">
         <v>5.1684000000000001</v>
       </c>
       <c r="I18">
-        <f>H18^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>2.989308556273552</v>
       </c>
     </row>
@@ -7995,28 +8297,28 @@
         <v>6.0069999999999997</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.4250000000000007</v>
       </c>
       <c r="C19">
         <v>5.5701000000000001</v>
       </c>
       <c r="D19">
-        <f>C19^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.1422591153980535</v>
       </c>
       <c r="F19">
         <v>8.3070000000000004</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.2370000000000001</v>
       </c>
       <c r="H19">
         <v>5.2830000000000004</v>
       </c>
       <c r="I19">
-        <f>H19^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.0333352158208609</v>
       </c>
     </row>
@@ -8025,28 +8327,28 @@
         <v>6.1040000000000001</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5220000000000002</v>
       </c>
       <c r="C20">
         <v>5.6685999999999996</v>
       </c>
       <c r="D20">
-        <f>C20^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.1791953042150967</v>
       </c>
       <c r="F20">
         <v>8.4019999999999992</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.331999999999999</v>
       </c>
       <c r="H20">
         <v>5.3780000000000001</v>
       </c>
       <c r="I20">
-        <f>H20^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.0695911348458544</v>
       </c>
     </row>
@@ -8055,28 +8357,28 @@
         <v>6.2050000000000001</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.6230000000000011</v>
       </c>
       <c r="C21">
         <v>5.7691999999999997</v>
       </c>
       <c r="D21">
-        <f>C21^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.2166987964014284</v>
       </c>
       <c r="F21">
         <v>8.4979999999999993</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.427999999999999</v>
       </c>
       <c r="H21">
         <v>5.4752000000000001</v>
       </c>
       <c r="I21">
-        <f>H21^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.1064663856427717</v>
       </c>
     </row>
@@ -8085,28 +8387,28 @@
         <v>6.3079999999999998</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.7259999999999991</v>
       </c>
       <c r="C22">
         <v>5.8657000000000004</v>
       </c>
       <c r="D22">
-        <f>C22^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.2524694916181072</v>
       </c>
       <c r="F22">
         <v>8.6059999999999999</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.5359999999999996</v>
       </c>
       <c r="H22">
         <v>5.5861000000000001</v>
       </c>
       <c r="I22">
-        <f>H22^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.1482736222576038</v>
       </c>
     </row>
@@ -8115,28 +8417,28 @@
         <v>6.4020000000000001</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.82</v>
       </c>
       <c r="C23">
         <v>5.9695</v>
       </c>
       <c r="D23">
-        <f>C23^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.2907278825448167</v>
       </c>
       <c r="F23">
         <v>8.7040000000000006</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.6340000000000003</v>
       </c>
       <c r="H23">
         <v>5.6864999999999997</v>
       </c>
       <c r="I23">
-        <f>H23^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.1858845147131558</v>
       </c>
     </row>
@@ -8145,28 +8447,28 @@
         <v>6.508</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.9260000000000002</v>
       </c>
       <c r="C24">
         <v>6.0784000000000002</v>
       </c>
       <c r="D24">
-        <f>C24^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.3306284246566542</v>
       </c>
       <c r="F24">
         <v>8.8030000000000008</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.7330000000000005</v>
       </c>
       <c r="H24">
         <v>5.7862999999999998</v>
       </c>
       <c r="I24">
-        <f>H24^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.2230518912575952</v>
       </c>
     </row>
@@ -8175,28 +8477,28 @@
         <v>6.7560000000000002</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.1739999999999995</v>
       </c>
       <c r="C25">
         <v>6.2938000000000001</v>
       </c>
       <c r="D25">
-        <f>C25^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.4088557616907988</v>
       </c>
       <c r="F25">
         <v>8.9</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.83</v>
       </c>
       <c r="H25">
         <v>5.8887</v>
       </c>
       <c r="I25">
-        <f>H25^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.2609661184273255</v>
       </c>
     </row>
@@ -8205,28 +8507,28 @@
         <v>6.8</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.218</v>
       </c>
       <c r="C26">
         <v>6.3414999999999999</v>
       </c>
       <c r="D26">
-        <f>C26^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.4260576341926599</v>
       </c>
       <c r="F26">
         <v>9.01</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.94</v>
       </c>
       <c r="H26">
         <v>5.9970999999999997</v>
       </c>
       <c r="I26">
-        <f>H26^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.3008632088330221</v>
       </c>
     </row>
@@ -8235,28 +8537,28 @@
         <v>7.0030000000000001</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.4209999999999994</v>
       </c>
       <c r="C27">
         <v>6.5552000000000001</v>
       </c>
       <c r="D27">
-        <f>C27^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.5026007075855841</v>
       </c>
       <c r="F27">
         <v>9.1</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.0299999999999994</v>
       </c>
       <c r="H27">
         <v>6.0814000000000004</v>
       </c>
       <c r="I27">
-        <f>H27^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.331724224377723</v>
       </c>
     </row>
@@ -8265,28 +8567,28 @@
         <v>7.2409999999999997</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.6589999999999989</v>
       </c>
       <c r="C28">
         <v>6.7960000000000003</v>
       </c>
       <c r="D28">
-        <f>C28^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.5878607584374302</v>
       </c>
       <c r="F28">
         <v>9.2050000000000001</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.1349999999999998</v>
       </c>
       <c r="H28">
         <v>6.1881000000000004</v>
       </c>
       <c r="I28">
-        <f>H28^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.3705818837497095</v>
       </c>
     </row>
@@ -8295,28 +8597,28 @@
         <v>7.5119999999999996</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.93</v>
       </c>
       <c r="C29">
         <v>7.0845000000000002</v>
       </c>
       <c r="D29">
-        <f>C29^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.6886954760292237</v>
       </c>
       <c r="F29">
         <v>9.3070000000000004</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.2370000000000001</v>
       </c>
       <c r="H29">
         <v>6.2964000000000002</v>
       </c>
       <c r="I29">
-        <f>H29^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.4097945072145222</v>
       </c>
     </row>
@@ -8325,28 +8627,28 @@
         <v>7.7560000000000002</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.173999999999999</v>
       </c>
       <c r="C30">
         <v>7.3422000000000001</v>
       </c>
       <c r="D30">
-        <f>C30^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.777613081130867</v>
       </c>
       <c r="F30">
         <v>9.3889999999999993</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.3189999999999991</v>
       </c>
       <c r="H30">
         <v>6.3804999999999996</v>
       </c>
       <c r="I30">
-        <f>H30^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.4400900308260653</v>
       </c>
     </row>
@@ -8355,28 +8657,28 @@
         <v>8.0489999999999995</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.466999999999999</v>
       </c>
       <c r="C31">
         <v>7.6543999999999999</v>
       </c>
       <c r="D31">
-        <f>C31^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>3.8839542215049447</v>
       </c>
       <c r="F31">
         <v>9.5030000000000001</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.4329999999999998</v>
       </c>
       <c r="H31">
         <v>6.5003000000000002</v>
       </c>
       <c r="I31">
-        <f>H31^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.4830170495749351</v>
       </c>
     </row>
@@ -8385,28 +8687,28 @@
         <v>8.5370000000000008</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.955000000000002</v>
       </c>
       <c r="C32">
         <v>8.2340999999999998</v>
       </c>
       <c r="D32">
-        <f>C32^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>4.0776576249797785</v>
       </c>
       <c r="F32">
         <v>9.6620000000000008</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.5920000000000005</v>
       </c>
       <c r="H32">
         <v>6.6643999999999997</v>
       </c>
       <c r="I32">
-        <f>H32^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.5413922875186925</v>
       </c>
     </row>
@@ -8415,28 +8717,28 @@
         <v>9.0649999999999995</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.483000000000001</v>
       </c>
       <c r="C33">
         <v>9.0761000000000003</v>
       </c>
       <c r="D33">
-        <f>C33^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>4.3511045102989634</v>
       </c>
       <c r="F33">
         <v>9.7550000000000008</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.6850000000000005</v>
       </c>
       <c r="H33">
         <v>6.7628000000000004</v>
       </c>
       <c r="I33">
-        <f>H33^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.5761662151836187</v>
       </c>
     </row>
@@ -8445,28 +8747,28 @@
         <v>9.5489999999999995</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.966999999999999</v>
       </c>
       <c r="C34">
         <v>10.1776</v>
       </c>
       <c r="D34">
-        <f>C34^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>4.6963838452932141</v>
       </c>
       <c r="F34">
         <v>10.012</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.9420000000000002</v>
       </c>
       <c r="H34">
         <v>7.0326000000000004</v>
       </c>
       <c r="I34">
-        <f>H34^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.670658182680941</v>
       </c>
     </row>
@@ -8475,28 +8777,28 @@
         <v>10.076000000000001</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.494</v>
       </c>
       <c r="C35">
         <v>12.156000000000001</v>
       </c>
       <c r="D35">
-        <f>C35^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>5.2868111135782048</v>
       </c>
       <c r="F35">
         <v>10.27</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.199999999999999</v>
       </c>
       <c r="H35">
         <v>7.3014000000000001</v>
       </c>
       <c r="I35">
-        <f>H35^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.7636054982797789</v>
       </c>
     </row>
@@ -8505,28 +8807,28 @@
         <v>10.494999999999999</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12.913</v>
       </c>
       <c r="C36">
         <v>14.525</v>
       </c>
       <c r="D36">
-        <f>C36^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>5.9531125583287441</v>
       </c>
       <c r="F36">
         <v>10.502000000000001</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.432</v>
       </c>
       <c r="H36">
         <v>7.5517000000000003</v>
       </c>
       <c r="I36">
-        <f>H36^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.8491350818076762</v>
       </c>
     </row>
@@ -8535,28 +8837,28 @@
         <v>10.763</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13.181000000000001</v>
       </c>
       <c r="C37">
         <v>16.954999999999998</v>
       </c>
       <c r="D37">
-        <f>C37^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>6.5998165314778401</v>
       </c>
       <c r="F37">
         <v>10.775</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.705</v>
       </c>
       <c r="H37">
         <v>7.8498999999999999</v>
       </c>
       <c r="I37">
-        <f>H37^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>3.9498088891140322</v>
       </c>
     </row>
@@ -8565,28 +8867,28 @@
         <v>11.026</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13.443999999999999</v>
       </c>
       <c r="C38">
         <v>21.56</v>
       </c>
       <c r="D38">
-        <f>C38^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>7.7463866610619565</v>
       </c>
       <c r="F38">
         <v>11.004</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.933999999999999</v>
       </c>
       <c r="H38">
         <v>8.1267999999999994</v>
       </c>
       <c r="I38">
-        <f>H38^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>4.0421557915694759</v>
       </c>
     </row>
@@ -8595,28 +8897,28 @@
         <v>11.138999999999999</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13.556999999999999</v>
       </c>
       <c r="C39">
         <v>47.502000000000002</v>
       </c>
       <c r="D39">
-        <f>C39^(2/3)</f>
+        <f t="shared" si="0"/>
         <v>13.116196977075232</v>
       </c>
       <c r="F39">
         <v>11.488</v>
       </c>
       <c r="G39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.417999999999999</v>
       </c>
       <c r="H39">
         <v>8.8444000000000003</v>
       </c>
       <c r="I39">
-        <f>H39^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>4.2767341114769204</v>
       </c>
     </row>
@@ -8625,14 +8927,14 @@
         <v>12.01</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.94</v>
       </c>
       <c r="H40">
         <v>9.9</v>
       </c>
       <c r="I40">
-        <f>H40^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>4.6105931042857726</v>
       </c>
     </row>
@@ -8641,14 +8943,14 @@
         <v>12.505000000000001</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12.435</v>
       </c>
       <c r="H41">
         <v>11.555</v>
       </c>
       <c r="I41">
-        <f>H41^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>5.1110873104156678</v>
       </c>
     </row>
@@ -8657,14 +8959,14 @@
         <v>12.756</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12.686</v>
       </c>
       <c r="H42">
         <v>12.888</v>
       </c>
       <c r="I42">
-        <f>H42^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>5.4969740269448382</v>
       </c>
     </row>
@@ -8673,14 +8975,14 @@
         <v>13.004</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12.933999999999999</v>
       </c>
       <c r="H43">
         <v>14.4</v>
       </c>
       <c r="I43">
-        <f>H43^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>5.9189089783931275</v>
       </c>
     </row>
@@ -8689,14 +8991,14 @@
         <v>13.297000000000001</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13.227</v>
       </c>
       <c r="H44">
         <v>17.317</v>
       </c>
       <c r="I44">
-        <f>H44^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>6.6934255624657863</v>
       </c>
     </row>
@@ -8705,14 +9007,14 @@
         <v>13.512</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13.442</v>
       </c>
       <c r="H45">
         <v>21.3</v>
       </c>
       <c r="I45">
-        <f>H45^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>7.6839831226550981</v>
       </c>
     </row>
@@ -8721,14 +9023,14 @@
         <v>13.742000000000001</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13.672000000000001</v>
       </c>
       <c r="H46">
         <v>24.617000000000001</v>
       </c>
       <c r="I46">
-        <f>H46^(2/3)</f>
+        <f t="shared" si="1"/>
         <v>8.4623324657175534</v>
       </c>
     </row>
@@ -8747,7 +9049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="D12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -8765,10 +9067,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A1" s="4">
+      <c r="A1" s="5">
         <v>365</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" t="s">
         <v>5</v>
       </c>
@@ -9663,7 +9965,7 @@
       <c r="H16">
         <v>11.167</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="4">
         <v>3.9</v>
       </c>
       <c r="J16">
@@ -10172,15 +10474,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.53125" customWidth="1"/>
-    <col min="2" max="2" width="16.86328125" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.19921875" customWidth="1"/>
+    <col min="2" max="2" width="24.53125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.59765625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="16.265625" customWidth="1"/>
@@ -10193,25 +10495,25 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="4">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6">
         <v>365</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -10310,22 +10612,22 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="4">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6">
         <v>492</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -10345,7 +10647,7 @@
         <v>12.608000000000001</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:B24" si="1">A18-2.418</f>
+        <f t="shared" ref="B18:B22" si="1">A18-2.418</f>
         <v>10.190000000000001</v>
       </c>
       <c r="C18">
@@ -10400,22 +10702,22 @@
         <v>10.53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="4">
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="6">
         <v>546</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -10426,7 +10728,7 @@
         <f>A28-2.418</f>
         <v>8.7489999999999988</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>3.9</v>
       </c>
     </row>
@@ -10438,7 +10740,7 @@
         <f t="shared" ref="B29:B35" si="2">A29-2.418</f>
         <v>8.9720000000000013</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -10521,5 +10823,11 @@
     <mergeCell ref="A26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding in outline for Final Report
</commit_message>
<xml_diff>
--- a/Ionization of Mercury/IonizationofMercury.xlsx
+++ b/Ionization of Mercury/IonizationofMercury.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4290" windowHeight="5415" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4290" windowHeight="5415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>Voltage (V)</t>
   </si>
@@ -89,6 +89,61 @@
   <si>
     <t>Current [mA*10^-9] (0.05 mA*10^-9)</t>
   </si>
+  <si>
+    <t>Extinctiion potentials</t>
+  </si>
+  <si>
+    <r>
+      <t>Expected Value [V] (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±0.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Wavelength [nm] (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Experimental Value [V] (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>±0.1)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -99,10 +154,18 @@
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -158,6 +221,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7481,6 +7547,22 @@
 </table>
 </file>
 
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A39:C42" totalsRowShown="0">
+  <autoFilter ref="A39:C42">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Wavelength [nm] (±2)"/>
+    <tableColumn id="2" name="Expected Value [V] (±0.1)"/>
+    <tableColumn id="3" name="Experimental Value [V] (±0.1)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9049,7 +9131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
+    <sheetView topLeftCell="C31" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -10472,10 +10554,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10496,11 +10578,11 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>365</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -10613,11 +10695,11 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="6">
+      <c r="A15" s="7">
         <v>492</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -10703,11 +10785,11 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="6">
+      <c r="A26" s="7">
         <v>546</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
@@ -10816,18 +10898,71 @@
         <v>11.1</v>
       </c>
     </row>
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A38" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>365</v>
+      </c>
+      <c r="B40">
+        <v>9.6</v>
+      </c>
+      <c r="C40">
+        <v>9.516</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>492</v>
+      </c>
+      <c r="B41">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C41">
+        <v>9.1660000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>546</v>
+      </c>
+      <c r="B42">
+        <v>7.9</v>
+      </c>
+      <c r="C42">
+        <v>8.0549999999999997</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A38:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>